<commit_message>
Avance en documento, gráficas de resumen de resultados
</commit_message>
<xml_diff>
--- a/Datos/Configuración 1/ResultadosCSV/ResultadosCSV conf 1.xlsx
+++ b/Datos/Configuración 1/ResultadosCSV/ResultadosCSV conf 1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulianDavid\Desktop\Andes\Semestre VI\Infraestructura Computacional\Caso 3\srv202010-fuentes\Caso3_Infracomp_Servidor\Datos\Configuración 1\ResultadosCSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF43CCA-A6E8-4663-B88A-6D4730EEB87D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681E5354-22A4-4FAE-899D-3F2F1D705CB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{4E5A8887-101A-4BA7-951F-C890C9AFB85B}"/>
   </bookViews>
@@ -6598,13 +6598,13 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>548640</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>55245</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>567690</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>55245</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6931,8 +6931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FACDF68C-0F42-4FDF-9DED-6D008DA0B733}">
   <dimension ref="A1:P4001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7123,7 +7123,7 @@
         <v>#N/A</v>
       </c>
       <c r="K6" s="1">
-        <f t="shared" ref="J6:L6" si="3">_xlfn.MODE.SNGL(K13:K412)</f>
+        <f t="shared" ref="K6:L6" si="3">_xlfn.MODE.SNGL(K13:K412)</f>
         <v>0</v>
       </c>
       <c r="L6" s="1">
@@ -7160,7 +7160,7 @@
         <v>1.0398402827356741E-3</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" ref="J7:L7" si="4">_xlfn.VAR.S(K13:K412)</f>
+        <f t="shared" ref="K7:L7" si="4">_xlfn.VAR.S(K13:K412)</f>
         <v>0</v>
       </c>
       <c r="L7" s="1">
@@ -7342,7 +7342,7 @@
         <v>0.52586220806701056</v>
       </c>
       <c r="K13">
-        <f t="shared" ref="J13:L13" si="6">(D2+D402+D802+D1202+D1602+D2002+D2402+D2802+D3202+D3602)/10</f>
+        <f t="shared" ref="K13:L13" si="6">(D2+D402+D802+D1202+D1602+D2002+D2402+D2802+D3202+D3602)/10</f>
         <v>0</v>
       </c>
       <c r="L13" s="5">

</xml_diff>